<commit_message>
a lot of code
</commit_message>
<xml_diff>
--- a/iban-name-check-async-impl/src/test/resources/excel/file.xlsx
+++ b/iban-name-check-async-impl/src/test/resources/excel/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sashankasamantray/my_projects/backend/sparkle-demo/iban-name-check/iban-name-check-async-impl/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EC84D2-74C4-BD4E-BBB8-556CD63B9765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D94C1A-2E7D-BF42-9145-D504CBD4AD41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" xr2:uid="{1038183B-3D39-2A42-9DB8-92BC73C0F8B4}"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{1038183B-3D39-2A42-9DB8-92BC73C0F8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Rekeningnummer</t>
   </si>
@@ -41,40 +41,64 @@
     <t>Naam rekeninghouder</t>
   </si>
   <si>
-    <t>NL19RABO233113123</t>
-  </si>
-  <si>
-    <t>Donald duck</t>
-  </si>
-  <si>
-    <t>NL19RABO233113124</t>
-  </si>
-  <si>
-    <t>Luffy Monkey</t>
-  </si>
-  <si>
-    <t>NL19RABO233113125</t>
-  </si>
-  <si>
-    <t>Zoro Roronoa</t>
-  </si>
-  <si>
-    <t>NL19RABO233113126</t>
-  </si>
-  <si>
-    <t>Abel Jansen</t>
-  </si>
-  <si>
-    <t>NL19RABO233113127</t>
-  </si>
-  <si>
-    <t>R. anuradaha</t>
-  </si>
-  <si>
-    <t>NL19RABO233113128</t>
-  </si>
-  <si>
-    <t>H. Groot</t>
+    <t>NL86RABO6333227641</t>
+  </si>
+  <si>
+    <t>Sally Snozcumber</t>
+  </si>
+  <si>
+    <t>NL06ABNA5558304928</t>
+  </si>
+  <si>
+    <t>Roy Olsson</t>
+  </si>
+  <si>
+    <t>NL36INGB2682297498</t>
+  </si>
+  <si>
+    <t>Barry Grey</t>
+  </si>
+  <si>
+    <t>NL10RABO9837080566</t>
+  </si>
+  <si>
+    <t>Chloe Donaldson</t>
+  </si>
+  <si>
+    <t>NL89INGB6034837898</t>
+  </si>
+  <si>
+    <t>Alison Blackman</t>
+  </si>
+  <si>
+    <t>NL57ABNA2454554658</t>
+  </si>
+  <si>
+    <t>Gemma Parkes</t>
+  </si>
+  <si>
+    <t>NL86INGB4110487447</t>
+  </si>
+  <si>
+    <t>Suzanne Blast</t>
+  </si>
+  <si>
+    <t>NL75ABNA9372718300</t>
+  </si>
+  <si>
+    <t>Sally Lakeman</t>
+  </si>
+  <si>
+    <t>NL23RABO5299017782</t>
+  </si>
+  <si>
+    <t>Hannah Connor</t>
+  </si>
+  <si>
+    <t>NL22ABNA5206019070</t>
+  </si>
+  <si>
+    <t>Morwenna Zeus</t>
   </si>
 </sst>
 </file>
@@ -127,13 +151,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -450,75 +474,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2993BB76-FCF7-CF4A-A795-6147B08C0CCA}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>